<commit_message>
Finacials and Transactions: 02/28/2021
</commit_message>
<xml_diff>
--- a/2021-sgfdevs-journal.xlsx
+++ b/2021-sgfdevs-journal.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -95,10 +95,76 @@
     <t>01/06/2021</t>
   </si>
   <si>
+    <t>02/01/2021</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>Pillar Insurance Springfield</t>
+  </si>
+  <si>
+    <t>Check               2001</t>
+  </si>
+  <si>
+    <t>Devs:Devs Insurance</t>
+  </si>
+  <si>
+    <t>02/02/2021</t>
+  </si>
+  <si>
+    <t>02/04/2021</t>
+  </si>
+  <si>
+    <t>AMAZON WEB SERVICES DBT CRD 2058 02/04/21 DBU05BHI</t>
+  </si>
+  <si>
+    <t>02/05/2021</t>
+  </si>
+  <si>
+    <t>02/08/2021</t>
+  </si>
+  <si>
+    <t>NAME.COM, INC DBT CRD 1221 02/06/21 DBH791RU</t>
+  </si>
+  <si>
+    <t>02/11/2021</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Self Interactive</t>
+  </si>
+  <si>
+    <t>Paid via QuickBooks Payments: Payment ID aoz5yxgx</t>
+  </si>
+  <si>
+    <t>Undeposited Funds</t>
+  </si>
+  <si>
+    <t>Accounts Receivable (A/R)</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>System-recorded deposit for QuickBooks Payments</t>
+  </si>
+  <si>
+    <t>QuickBooks Payments</t>
+  </si>
+  <si>
+    <t>System-recorded fee for QuickBooks Payments. Fee-name: DiscountRateFee, fee-type: Daily.</t>
+  </si>
+  <si>
+    <t>Devs:Devs Payment Fees (Intuit)</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Monday, Feb 08, 2021 04:32:33 PM GMT-8</t>
+    <t>Tuesday, Mar 09, 2021 06:08:13 AM GMT-8</t>
   </si>
   <si>
     <t>Springfield Devs</t>
@@ -107,7 +173,7 @@
     <t>Journal</t>
   </si>
   <si>
-    <t>January 2021</t>
+    <t>January - February, 2021</t>
   </si>
 </sst>
 </file>
@@ -217,7 +283,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -229,15 +295,15 @@
     <col min="4" max="4" width="8.59375" customWidth="true"/>
     <col min="5" max="5" width="7.734375" customWidth="true"/>
     <col min="6" max="6" width="32.65625" customWidth="true"/>
-    <col min="7" max="7" width="55.859375" customWidth="true"/>
-    <col min="8" max="8" width="24.921875" customWidth="true"/>
-    <col min="9" max="9" width="8.59375" customWidth="true"/>
-    <col min="10" max="10" width="8.59375" customWidth="true"/>
+    <col min="7" max="7" width="76.484375" customWidth="true"/>
+    <col min="8" max="8" width="27.5" customWidth="true"/>
+    <col min="9" max="9" width="9.453125" customWidth="true"/>
+    <col min="10" max="10" width="9.453125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -251,7 +317,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -265,7 +331,7 @@
     </row>
     <row r="3">
       <c r="A3" s="9" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -651,33 +717,631 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s" s="6">
+      <c r="B34" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="I34" t="n" s="5">
-        <v>120.27</v>
-      </c>
-      <c r="J34" t="n" s="5">
-        <v>120.27</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="7" t="s">
+      <c r="C34" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" t="n" s="4">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="H35" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="I35" t="n" s="4">
+        <v>14.99</v>
+      </c>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36">
+      <c r="I36" t="n" s="5">
+        <v>14.99</v>
+      </c>
+      <c r="J36" t="n" s="5">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" t="n" s="4">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="H39" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="I39" t="n" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40">
+      <c r="I40" t="n" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="J40" t="n" s="5">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="J42" t="n" s="4">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="I43" t="n" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44">
+      <c r="I44" t="n" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="J44" t="n" s="5">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="C46" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-      <c r="J37"/>
+      <c r="D46" t="n" s="2">
+        <v>2001.0</v>
+      </c>
+      <c r="E46" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F46" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="H46" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" t="n" s="4">
+        <v>1148.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="H47" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="I47" t="n" s="4">
+        <v>1148.0</v>
+      </c>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48">
+      <c r="I48" t="n" s="5">
+        <v>1148.0</v>
+      </c>
+      <c r="J48" t="n" s="5">
+        <v>1148.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F50" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" t="n" s="4">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="I51" t="n" s="4">
+        <v>14.99</v>
+      </c>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52">
+      <c r="I52" t="n" s="5">
+        <v>14.99</v>
+      </c>
+      <c r="J52" t="n" s="5">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="C54" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F54" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="G54" s="2"/>
+      <c r="H54" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" t="n" s="4">
+        <v>10.22</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="I55" t="n" s="4">
+        <v>10.22</v>
+      </c>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56">
+      <c r="I56" t="n" s="5">
+        <v>10.22</v>
+      </c>
+      <c r="J56" t="n" s="5">
+        <v>10.22</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="C58" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F58" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="G58" s="2"/>
+      <c r="H58" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="I58" s="3"/>
+      <c r="J58" t="n" s="4">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="H59" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="I59" t="n" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60">
+      <c r="I60" t="n" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="J60" t="n" s="5">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="C62" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F62" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="G62" s="2"/>
+      <c r="H62" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="I62" s="3"/>
+      <c r="J62" t="n" s="4">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="I63" t="n" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64">
+      <c r="I64" t="n" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="J64" t="n" s="5">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="C66" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" t="n" s="4">
+        <v>232.48</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H67" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="I67" t="n" s="4">
+        <v>232.48</v>
+      </c>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68">
+      <c r="I68" t="n" s="5">
+        <v>232.48</v>
+      </c>
+      <c r="J68" t="n" s="5">
+        <v>232.48</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="C70" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F70" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G70" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H70" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I70" t="n" s="4">
+        <v>600.0</v>
+      </c>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="I71" s="3"/>
+      <c r="J71" t="n" s="4">
+        <v>600.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="I72" t="n" s="5">
+        <v>600.0</v>
+      </c>
+      <c r="J72" t="n" s="5">
+        <v>600.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="C74" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F74" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G74" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H74" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="I74" t="n" s="4">
+        <v>600.0</v>
+      </c>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F75" s="2"/>
+      <c r="G75" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H75" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="I75" s="3"/>
+      <c r="J75" t="n" s="4">
+        <v>600.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="I76" t="n" s="5">
+        <v>600.0</v>
+      </c>
+      <c r="J76" t="n" s="5">
+        <v>600.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="C78" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F78" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="G78" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H78" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" t="n" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F79" s="2"/>
+      <c r="G79" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H79" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="I79" t="n" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80">
+      <c r="I80" t="n" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="J80" t="n" s="5">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="6">
+        <v>49</v>
+      </c>
+      <c r="I82" t="n" s="5">
+        <v>2826.95</v>
+      </c>
+      <c r="J82" t="n" s="5">
+        <v>2826.95</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B85"/>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85"/>
+      <c r="J85"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="A85:J85"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>

</xml_diff>